<commit_message>
Modifying Countries Flag File
</commit_message>
<xml_diff>
--- a/Countries-Flag-URL-Icon.xlsx
+++ b/Countries-Flag-URL-Icon.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fedea\Desktop\Consultoria BI\Challenges\Onyx COVID\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fedea\Desktop\Prueba-Github\COVID-19-Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2A5B52-6F77-4C11-BB75-266663B582D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E64F34-76D6-44EA-8608-DBFD0844B7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{85ABF54D-4E09-48D8-A0C1-C431334870BF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="443">
   <si>
     <t>iso_code</t>
   </si>
@@ -1351,6 +1351,9 @@
   </si>
   <si>
     <t>https://www.countryflags.io/uy/flat/64.png</t>
+  </si>
+  <si>
+    <t>PRUEBA</t>
   </si>
 </sst>
 </file>
@@ -1713,10 +1716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A1A1C4-A94D-4EE1-9068-8288A05B6670}">
-  <dimension ref="A1:B222"/>
+  <dimension ref="A1:B223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="C197" sqref="C197"/>
+    <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
+      <selection activeCell="B223" sqref="B223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3495,6 +3498,14 @@
       </c>
       <c r="B222" s="1" t="s">
         <v>436</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>442</v>
+      </c>
+      <c r="B223">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>